<commit_message>
Se añaden modificaciones para las etiquetas FormInput, Button, HBox y VBox
</commit_message>
<xml_diff>
--- a/miscellaneous/Mapping MXML to Pug - BOL.xlsx
+++ b/miscellaneous/Mapping MXML to Pug - BOL.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\selene.estevez\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\selene.estevez\eclipse-workspace-mxml\com.softtek.mxml\miscellaneous\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Tag</t>
   </si>
@@ -47,9 +47,6 @@
     <t>label Fecha de Liquidación</t>
   </si>
   <si>
-    <t>label(id="lblEstado" data-i18n="medapp_estado.estado"): span(class="required")*</t>
-  </si>
-  <si>
     <t>label(id="lblNaturaleza" data-i18n="medapp_consultaNaturaleza_idReglaCorte.consultaNaturaleza_idReglaCorte")</t>
   </si>
   <si>
@@ -71,23 +68,116 @@
     <t>label(data-i18n="medapp_propiedadBase.propiedadBase" style="visibility: hidden")</t>
   </si>
   <si>
-    <t>Para la generación de código no se toman encuenta los atributos: paddingTop,  height, paddingBottom, direction ni width</t>
+    <t>mx:Button</t>
+  </si>
+  <si>
+    <t>&lt;mx:Button id="btnSi" label="Aceptar" styleName="btnSi"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mx:Button id="btnNo" label="No" click="cancelaAgregaTransaccion(event)" styleName="btnNo" width="75"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mx:Button id="txiFolioInstTrasp" width="45" height="30" label="{cmbNombreInstTrasp.selectedItem.folioInstitucion}" styleName="btnFolio"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mx:Button id="btnCancelarMultiple" label="Limpiar" enabled="false" click="construyeCancelacionMultiple()" styleName="btnLimpiar"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mx:Button id="btnAdd" toolTip="Agregar archivo" click="addFiles()" icon="@Embed('/images/fileUpload/add.png')" width="26"&gt;</t>
+  </si>
+  <si>
+    <t>button(type="button" id="btnSi") Aceptar</t>
+  </si>
+  <si>
+    <t>button(type="button" id="btnNo" title="click=cancelaAgregaTransaccion(event)") No</t>
+  </si>
+  <si>
+    <t>button(type="button" id="btnNo" title="click=cancelaAgregaTransaccion(event)") cmbNombreInstTrasp.selectedItem.folioInstitucion</t>
+  </si>
+  <si>
+    <t>button(type="button" id="btnCancelarMultiple" title="click=construyeCancelacionMultiple()" disabled) Limpiar</t>
+  </si>
+  <si>
+    <t>button(type="button" id="btnAdd" title="toolTip=Agregar archivo click=construyeCancelacionMultiple()" disabled) @Embed('/images/fileUpload/add.png')</t>
+  </si>
+  <si>
+    <t>&lt;mx:Button id="btnShowErrors" icon="@Embed('/images/fileUpload/next.png')" label="Muestra Errores" click="{this.currentState='st_results'}"&gt;</t>
+  </si>
+  <si>
+    <t>Para la generación de código no se toman encuenta los atributos: skin, width, height,  styleName, textAlign, borderColor, labelPlacement, buttonMode, useHandCursor, horizontalCenter, bottom, xmlns:mx, implements</t>
+  </si>
+  <si>
+    <t>button(type="button" id="btnShowErrors" title="click={this.currentState='st_results'}") Muestra Errores @Embed('/images/fileUpload/next.png')</t>
+  </si>
+  <si>
+    <t>mx:Hbox</t>
+  </si>
+  <si>
+    <t>&lt;mx:HBox id="hBoxTiposTraspaso" width="980" height="90%" horizontalAlign="center" verticalAlign="middle" horizontalScrollPolicy="off" styleName="containerTab" paddingBottom="15"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mx:HBox width="100%" height="100%"&gt;</t>
+  </si>
+  <si>
+    <t>div(id="hBoxTiposTraspaso" class="hBox")</t>
+  </si>
+  <si>
+    <t>div(class="hBox")</t>
+  </si>
+  <si>
+    <t>Para la generación de código no se toman en cuenta los atributos: width, paddingTop, verticalScrollPolicy, horizontalScrollPolicy, horizontalAlign, height, verticalAlign, horizontalGap, styleName, paddingBottom, paddingLeft, paddingRight, minHeight, xmlns:mx, xmlns:controls, xmlns:view, creationComplete, implements, xmlns:mate, right, xmlns:views, initialize, xmlns:maps, disabledOverlayAlpha</t>
+  </si>
+  <si>
+    <t>mx:Vbox</t>
+  </si>
+  <si>
+    <t>&lt;mx:VBox xmlns:mx="http://www.adobe.com/2006/mxml" verticalAlign="middle" horizontalAlign="center" width="90%" height="90%"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mx:VBox id="vBoxMain" width="0" height="0" horizontalAlign="center" visible="false" verticalAlign="middle" paddingTop="0" verticalGap="0"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mx:VBox id="vBoxDtg" width="100%" horizontalAlign="center" paddingTop="5"&gt;</t>
+  </si>
+  <si>
+    <t>div(class="vBox")</t>
+  </si>
+  <si>
+    <t>div(class="vBox" id="vBoxMain"  style="visibility: hidden")</t>
+  </si>
+  <si>
+    <t>div(class="vBox" id="vBoxDtg")</t>
+  </si>
+  <si>
+    <t>&lt;mx:HBox id="vBoxMain" width="0" height="0" horizontalAlign="center" visible="false" verticalAlign="middle" paddingTop="0" verticalGap="0"&gt;</t>
+  </si>
+  <si>
+    <t>div(class="hBox" id="vBoxMain"  style="visibility: hidden")</t>
+  </si>
+  <si>
+    <t>&lt;mx:VBox id="vBoxEmisionesIndeval" label="{resourceManager.getString('medapp','emisionesIndeval')}" width="100%" height="100%" horizontalScrollPolicy="off"&gt;</t>
+  </si>
+  <si>
+    <t>div(class="vBox" id="vBoxEmisionesIndeval")
+   label(data-i18n="medapp_emisionesIndeval.emisionesIndeval")</t>
+  </si>
+  <si>
+    <t>Para la generación de código no se toman en cuenta los atributos: xmlns:mx, width, height, paddingTop, verticalGap, horizontalAlign, verticalAlign, xmlns:viewCmp, xmlns:validatorCmp, xmlns:rm, xmlns:components, creationComplete, paddingBottom,  paddingLeft, xmlns:cmpView, xmlns:cmpViewRender, xmlns:cmpViewUpload, visible, x, y, xmlns:com, verticalScrollPolicy, paddingRight, initialize, horizontalScrollPolicy, xmlns:component, scroll, backgroundAlpha, backgroundColor, cornerRadius, xmlns:vista, left, right, xmlns:views, horizontalCenter, verticalCenter, xmlns:controls, xmlns:view, disabledOverlayAlpha, implements</t>
+  </si>
+  <si>
+    <t>Para la generación de código no se toman encuenta los atributos: paddingTop,  height, paddingBottom, direction, width</t>
+  </si>
+  <si>
+    <t>label(id="lblEstado" data-i18n="medapp_estado.estado")
+span(class="required") *</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -101,7 +191,24 @@
       <family val="3"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Consolas"/>
       <family val="3"/>
@@ -115,7 +222,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -210,52 +317,167 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -537,92 +759,241 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="129.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="123.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="70.21875" customWidth="1"/>
+    <col min="1" max="1" width="13.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="129.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="123.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.21875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="11.5546875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="27" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="33"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="33"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="33"/>
+    </row>
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="3"/>
+      <c r="B6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="13" t="s">
+      <c r="D6" s="34"/>
+    </row>
+    <row r="7" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
-      <c r="B3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="14"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="14"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
-      <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="14"/>
-    </row>
-    <row r="6" spans="1:4" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="15"/>
+      <c r="C7" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="6"/>
+      <c r="B8" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="33"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="6"/>
+      <c r="B9" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="33"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="6"/>
+      <c r="B10" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="33"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="6"/>
+      <c r="B11" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="33"/>
+    </row>
+    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="7"/>
+      <c r="B12" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="34"/>
+    </row>
+    <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="36"/>
+    </row>
+    <row r="15" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="3"/>
+      <c r="B15" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="37"/>
+    </row>
+    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="38" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="30"/>
+      <c r="B17" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D17" s="39"/>
+    </row>
+    <row r="18" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="30"/>
+      <c r="B18" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="39"/>
+    </row>
+    <row r="19" spans="1:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="31"/>
+      <c r="B19" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="8">
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="D16:D19"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="D2:D6"/>
+    <mergeCell ref="D7:D12"/>
+    <mergeCell ref="A7:A12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Se añaden modificaciones para Button y LinkButton
</commit_message>
<xml_diff>
--- a/miscellaneous/Mapping MXML to Pug - BOL.xlsx
+++ b/miscellaneous/Mapping MXML to Pug - BOL.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Tag</t>
   </si>
@@ -170,13 +170,40 @@
   <si>
     <t>label(id="lblEstado" data-i18n="medapp_estado.estado")
 span(class="required") *</t>
+  </si>
+  <si>
+    <t>mx:LinkButton</t>
+  </si>
+  <si>
+    <t>&lt;mx:LinkButton label="{resourceManager.getString('medapp','catalogoTipoValor')}" id="lblCatalogoTipoValor" click="{abrirVentana(event)}"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mx:LinkButton label="{resourceManager.getString('medapp','catalogoTipoValor')}" id="lblCatalogoTipoValor"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mx:LinkButton label="{resourceManager.getString('medapp','catalogoTipoValor')}" &gt;</t>
+  </si>
+  <si>
+    <t>a(href="#"): button(class="linkButton" type="button" id="lblCatalogoTipoValor" data-i18n="medapp_catalogoTipoValor.catalogoTipoValor" title="click={abrirVentana(event)")</t>
+  </si>
+  <si>
+    <t>a(href="#"): button(class="linkButton" type="button" id="lblCatalogoTipoValor" data-i18n="medapp_catalogoTipoValor.catalogoTipoValor")</t>
+  </si>
+  <si>
+    <t>a(href="#"): button(class="linkButton" type="button" data-i18n="medapp_catalogoTipoValor.catalogoTipoValor")</t>
+  </si>
+  <si>
+    <t>&lt;mx:Button id="btnShowErrors"  label="{resourceManager.getString('medapp','estado')}:" click="{this.currentState='st_results'}"&gt;</t>
+  </si>
+  <si>
+    <t>button(type="button" id="btnShowErrors" title="click={this.currentState='st_results'} icon=@Embed('/images/fileUpload/next.png')" data-i18n="medapp_estado.estado")</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,6 +240,13 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -372,27 +406,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -440,6 +456,27 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -450,6 +487,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -458,27 +504,38 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -759,241 +816,288 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="129.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="123.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="70.21875" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="11.5546875" style="4"/>
+    <col min="1" max="1" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="129.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="123.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.21875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="21" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="36" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="10" t="s">
+      <c r="A3" s="25"/>
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="33"/>
+      <c r="D3" s="37"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="10" t="s">
+      <c r="A4" s="25"/>
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="33"/>
+      <c r="D4" s="37"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="10" t="s">
+      <c r="A5" s="25"/>
+      <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="33"/>
+      <c r="D5" s="37"/>
     </row>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3"/>
-      <c r="B6" s="12" t="s">
+      <c r="A6" s="26"/>
+      <c r="B6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="34"/>
+      <c r="D6" s="38"/>
     </row>
     <row r="7" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="36" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
-      <c r="B8" s="16" t="s">
+      <c r="A8" s="40"/>
+      <c r="B8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="33"/>
+      <c r="D8" s="37"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
-      <c r="B9" s="16" t="s">
+      <c r="A9" s="40"/>
+      <c r="B9" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="33"/>
+      <c r="D9" s="37"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
-      <c r="B10" s="16" t="s">
+      <c r="A10" s="40"/>
+      <c r="B10" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="33"/>
+      <c r="D10" s="37"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
-      <c r="B11" s="16" t="s">
+      <c r="A11" s="40"/>
+      <c r="B11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="33"/>
-    </row>
-    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="7"/>
-      <c r="B12" s="18" t="s">
+      <c r="D11" s="37"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="40"/>
+      <c r="B12" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="37"/>
+    </row>
+    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="41"/>
+      <c r="B13" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C13" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="34"/>
-    </row>
-    <row r="13" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
+      <c r="D13" s="38"/>
+    </row>
+    <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B14" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C14" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="35" t="s">
+      <c r="D14" s="27" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="21" t="s">
+    <row r="15" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="25"/>
+      <c r="B15" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C15" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="36"/>
-    </row>
-    <row r="15" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="3"/>
-      <c r="B15" s="22" t="s">
+      <c r="D15" s="28"/>
+    </row>
+    <row r="16" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="26"/>
+      <c r="B16" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C16" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="37"/>
-    </row>
-    <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="29" t="s">
+      <c r="D16" s="29"/>
+    </row>
+    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B17" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C17" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="38" t="s">
+      <c r="D17" s="33" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="30"/>
-      <c r="B17" s="21" t="s">
+    <row r="18" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="31"/>
+      <c r="B18" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C18" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="39"/>
-    </row>
-    <row r="18" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="30"/>
-      <c r="B18" s="21" t="s">
+      <c r="D18" s="34"/>
+    </row>
+    <row r="19" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="31"/>
+      <c r="B19" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C19" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="39"/>
-    </row>
-    <row r="19" spans="1:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="31"/>
-      <c r="B19" s="19" t="s">
+      <c r="D19" s="34"/>
+    </row>
+    <row r="20" spans="1:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="32"/>
+      <c r="B20" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C20" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="40"/>
+      <c r="D20" s="35"/>
+    </row>
+    <row r="21" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="46"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="44"/>
+      <c r="B22" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="47"/>
+    </row>
+    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="45"/>
+      <c r="B23" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" s="48"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B24" s="50"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="D16:D19"/>
+  <mergeCells count="10">
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="D17:D20"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="D2:D6"/>
-    <mergeCell ref="D7:D12"/>
-    <mergeCell ref="A7:A12"/>
+    <mergeCell ref="D7:D13"/>
+    <mergeCell ref="A7:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Se añaden modificaciones para los tags Label, TextArea, TextInput, Label y Text
</commit_message>
<xml_diff>
--- a/miscellaneous/Mapping MXML to Pug - BOL.xlsx
+++ b/miscellaneous/Mapping MXML to Pug - BOL.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t>Tag</t>
   </si>
@@ -197,6 +197,118 @@
   </si>
   <si>
     <t>button(type="button" id="btnShowErrors" title="click={this.currentState='st_results'} icon=@Embed('/images/fileUpload/next.png')" data-i18n="medapp_estado.estado")</t>
+  </si>
+  <si>
+    <t>Para la generación de código no se toman en cuenta los atributos: width, selectable</t>
+  </si>
+  <si>
+    <t>mx:Text</t>
+  </si>
+  <si>
+    <t>&lt;mx:Text text="Nombre"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mx:Text text="{resourceManager.getString('medapp','idMercadoTitulo')}&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mx:Text text="Nombre" id="lblNombre"&gt;</t>
+  </si>
+  <si>
+    <t>label Nombre</t>
+  </si>
+  <si>
+    <t>label(id="lblNombre") Nombre</t>
+  </si>
+  <si>
+    <t>label(data-i18n="medapp_idMercadoTitulo.idMercadoTitulo")</t>
+  </si>
+  <si>
+    <t>mx:TextArea</t>
+  </si>
+  <si>
+    <t>&lt;mx:TextArea id="txaAlert" width="300" textAlign="center" wordWrap="true" selectable="false" editable="false" borderStyle="none&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mx:TextArea width="284" wordWrap="true" textAlign="center" selectable="false" editable="false" borderStyle="none" text="Ya existe un traspaso con estos datos. ¿Deseas continuar agregándolo?"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mx:TextArea editable="false" text="{this._errores.descripcionError}" fontWeight="bold"&gt;</t>
+  </si>
+  <si>
+    <t>textarea(id="textArea1" rows="4" cols="50" disabled)</t>
+  </si>
+  <si>
+    <t>textarea(rows="4" cols="50") Ya existe un traspaso con estos datos. ¿Deseas continuar agregándolo?</t>
+  </si>
+  <si>
+    <t>textarea(rows="4" cols="50" disabled) this._errores.descripcionError</t>
+  </si>
+  <si>
+    <t>Para la generación de código no se toman en cuenta los atributos: width, textAlign, wordWrap, selectable, borderStyle, height, htmlText, horizontalScrollPolicy, verticalScrollPolicy, fontWeight, borderThickness, paddingLeft, paddingBottom, paddingRight, paddingTop</t>
+  </si>
+  <si>
+    <t>mx:TextInput</t>
+  </si>
+  <si>
+    <t>&lt;mx:TextInput id="txiCantidad" restrict="0-9" maxChars="16" width="132" focusOut="{LiqUtils.generaFormato(txiCantidad)}"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mx:TextInput id="txtcuponVigente" enabled="false" width="55"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mx:TextInput restrict="0-9\-" change="validarInformacion(event)" keyUp="{refrescarEnter(event)}" keyDown="{manejaTab(event)}" focusOut="{focoFuera(event)}" disabledColor="{MedClsConstantes.COLOR_FONDO_DESHABILITADO_ADVANCED_DATAGRID}"&gt;</t>
+  </si>
+  <si>
+    <t>input(type="text" id="txiCantidad")</t>
+  </si>
+  <si>
+    <t>input(type="text" id="txtcuponVigente" disabled)</t>
+  </si>
+  <si>
+    <t>input(type="text")</t>
+  </si>
+  <si>
+    <t>Para la generación de código no se toman en cuenta los atributos: restrict, maxChars, width, focusOut, editable, change, text, textAlign, keyUp, keyDown, disabledColor, enter</t>
+  </si>
+  <si>
+    <t>Para la generación de código no se toman en cuenta los atributos: styleName, width, verticalScrollPolicy, horizontalScrollPolicy, paddingBottom, layout, horizontalAlign, paddingLeft, paddingRight, xmlns:mx, height, paddingTop, xmlns:cmpView, verticalAlign, creationComplete, resizeEffect, titleStyleName</t>
+  </si>
+  <si>
+    <t>mx:Panel</t>
+  </si>
+  <si>
+    <t>&lt;mx:Panel styleName="containerGenerico" title="TIPO DE OPERACIÓN" width="60%" verticalScrollPolicy="off" horizontalScrollPolicy="off" paddingBottom="5"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;mx:Panel title="{resourceManager.getString('medapp','filtro')}" id="filtro" resizeEffect="efecto"&gt;</t>
+  </si>
+  <si>
+    <t>div(class="panel")
+   div(class="panelTitle")
+      p TIPO DE OPERACIÓN
+   div(class="panelContent")
+      input(type="text")
+      input(type="text")
+      input(type="text")</t>
+  </si>
+  <si>
+    <t>div(class="panel" id="filtro")
+   div(class="panelTitle")
+      p(data-i18n="medapp_filtro.filtro")
+   div(class="panelContent")
+      input(type="text")
+      input(type="text")
+      input(type="text")</t>
+  </si>
+  <si>
+    <t>&lt;mx:Panel xmlns:mx="http://www.adobe.com/2006/mxml" width="1000" height="475" paddingTop="10" mlns:cmpView="mx.com.accival.utils.indeval.traspasos.view.*" layout="vertical" horizontalAlign="center" verticalAlign="middle" creationComplete="init(event)"&gt;</t>
+  </si>
+  <si>
+    <t>div(class="panel")     
+   div(class="panelContent")
+      input(type="text")
+      input(type="text")
+      input(type="text")</t>
   </si>
 </sst>
 </file>
@@ -406,14 +518,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -423,21 +533,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -459,6 +563,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -468,6 +576,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -495,47 +639,48 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -816,288 +961,432 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="129.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="129.109375" style="55" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="123.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="70.21875" style="1" customWidth="1"/>
     <col min="5" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="13" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="18" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="21" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A3" s="25"/>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="19"/>
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="37"/>
+      <c r="D3" s="22"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="25"/>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="19"/>
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="37"/>
+      <c r="D4" s="22"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="25"/>
-      <c r="B5" s="4" t="s">
+      <c r="A5" s="19"/>
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="37"/>
+      <c r="D5" s="22"/>
     </row>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="26"/>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="20"/>
+      <c r="B6" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="38"/>
+      <c r="D6" s="23"/>
     </row>
     <row r="7" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="39" t="s">
+      <c r="A7" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="21" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="40"/>
-      <c r="B8" s="10" t="s">
+      <c r="A8" s="25"/>
+      <c r="B8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="37"/>
+      <c r="D8" s="22"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="40"/>
-      <c r="B9" s="10" t="s">
+      <c r="A9" s="25"/>
+      <c r="B9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="37"/>
+      <c r="D9" s="22"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="40"/>
-      <c r="B10" s="10" t="s">
+      <c r="A10" s="25"/>
+      <c r="B10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="37"/>
+      <c r="D10" s="22"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="40"/>
-      <c r="B11" s="10" t="s">
+      <c r="A11" s="25"/>
+      <c r="B11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="37"/>
+      <c r="D11" s="22"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="40"/>
-      <c r="B12" s="10" t="s">
+      <c r="A12" s="25"/>
+      <c r="B12" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="37"/>
+      <c r="D12" s="22"/>
     </row>
     <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="41"/>
-      <c r="B13" s="12" t="s">
+      <c r="A13" s="26"/>
+      <c r="B13" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="38"/>
+      <c r="D13" s="23"/>
     </row>
     <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="27" t="s">
+      <c r="D14" s="33" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="25"/>
-      <c r="B15" s="15" t="s">
+      <c r="A15" s="19"/>
+      <c r="B15" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="28"/>
+      <c r="D15" s="34"/>
     </row>
     <row r="16" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="26"/>
-      <c r="B16" s="16" t="s">
+      <c r="A16" s="20"/>
+      <c r="B16" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="29"/>
+      <c r="D16" s="35"/>
     </row>
     <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="39" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="31"/>
-      <c r="B18" s="15" t="s">
+      <c r="A18" s="37"/>
+      <c r="B18" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="34"/>
+      <c r="D18" s="40"/>
     </row>
     <row r="19" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="31"/>
-      <c r="B19" s="15" t="s">
+      <c r="A19" s="37"/>
+      <c r="B19" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="34"/>
+      <c r="D19" s="40"/>
     </row>
     <row r="20" spans="1:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="32"/>
-      <c r="B20" s="13" t="s">
+      <c r="A20" s="38"/>
+      <c r="B20" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="22" t="s">
+      <c r="C20" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="35"/>
+      <c r="D20" s="41"/>
     </row>
     <row r="21" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="43" t="s">
+      <c r="A21" s="27" t="s">
         <v>48</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="46"/>
+      <c r="D21" s="30"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="44"/>
-      <c r="B22" s="4" t="s">
+      <c r="A22" s="28"/>
+      <c r="B22" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="47"/>
+      <c r="D22" s="31"/>
     </row>
     <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="45"/>
-      <c r="B23" s="49" t="s">
+      <c r="A23" s="29"/>
+      <c r="B23" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="48"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B24" s="50"/>
+      <c r="D23" s="32"/>
+    </row>
+    <row r="24" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="19"/>
+      <c r="B25" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="22"/>
+    </row>
+    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="20"/>
+      <c r="B26" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="23"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" s="39" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="19"/>
+      <c r="B28" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" s="40"/>
+    </row>
+    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="20"/>
+      <c r="B29" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" s="41"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="42" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="19"/>
+      <c r="B31" s="53" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" s="43"/>
+    </row>
+    <row r="32" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="20"/>
+      <c r="B32" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" s="44"/>
+    </row>
+    <row r="33" spans="1:4" ht="72.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A33" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="72.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A34" s="28"/>
+      <c r="B34" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" s="47" t="s">
+        <v>86</v>
+      </c>
+      <c r="D34" s="22"/>
+    </row>
+    <row r="35" spans="1:4" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="29"/>
+      <c r="B35" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" s="23"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D38" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="18">
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="D7:D13"/>
+    <mergeCell ref="A7:A13"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="A24:A26"/>
     <mergeCell ref="A21:A23"/>
     <mergeCell ref="D21:D23"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="D14:D16"/>
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="D17:D20"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="D2:D6"/>
-    <mergeCell ref="D7:D13"/>
-    <mergeCell ref="A7:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Generación de componentes para el proyecto gulp-pug-sass-ts a partir de mxml
</commit_message>
<xml_diff>
--- a/miscellaneous/Mapping MXML to Pug - BOL.xlsx
+++ b/miscellaneous/Mapping MXML to Pug - BOL.xlsx
@@ -360,12 +360,18 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="13">
@@ -567,13 +573,46 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -585,22 +624,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -621,15 +660,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -648,38 +678,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -963,14 +969,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="129.109375" style="55" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="129.109375" style="28" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="123.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="70.21875" style="1" customWidth="1"/>
     <col min="5" max="16384" width="11.5546875" style="1"/>
@@ -991,7 +997,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="29" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1000,52 +1006,52 @@
       <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="32" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A3" s="19"/>
+      <c r="A3" s="30"/>
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="22"/>
+      <c r="D3" s="33"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="19"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="22"/>
+      <c r="D4" s="33"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="19"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="22"/>
+      <c r="D5" s="33"/>
     </row>
     <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="20"/>
-      <c r="B6" s="46" t="s">
+      <c r="A6" s="31"/>
+      <c r="B6" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="23"/>
+      <c r="D6" s="34"/>
     </row>
     <row r="7" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="35" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="6" t="s">
@@ -1054,150 +1060,150 @@
       <c r="C7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="32" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="25"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="22"/>
+      <c r="D8" s="33"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="25"/>
+      <c r="A9" s="36"/>
       <c r="B9" s="7" t="s">
         <v>17</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="22"/>
+      <c r="D9" s="33"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="25"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="22"/>
+      <c r="D10" s="33"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="25"/>
+      <c r="A11" s="36"/>
       <c r="B11" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="22"/>
+      <c r="D11" s="33"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="25"/>
+      <c r="A12" s="36"/>
       <c r="B12" s="7" t="s">
         <v>55</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="22"/>
+      <c r="D12" s="33"/>
     </row>
     <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="26"/>
+      <c r="A13" s="37"/>
       <c r="B13" s="8" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="23"/>
+      <c r="D13" s="34"/>
     </row>
     <row r="14" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="21" t="s">
         <v>29</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="33" t="s">
+      <c r="D14" s="44" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="19"/>
-      <c r="B15" s="49" t="s">
+      <c r="A15" s="30"/>
+      <c r="B15" s="22" t="s">
         <v>41</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="34"/>
+      <c r="D15" s="45"/>
     </row>
     <row r="16" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="20"/>
-      <c r="B16" s="50" t="s">
+      <c r="A16" s="31"/>
+      <c r="B16" s="23" t="s">
         <v>30</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="35"/>
+      <c r="D16" s="46"/>
     </row>
     <row r="17" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="53" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="21" t="s">
         <v>35</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="39" t="s">
+      <c r="D17" s="47" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="37"/>
-      <c r="B18" s="49" t="s">
+      <c r="A18" s="54"/>
+      <c r="B18" s="22" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="40"/>
+      <c r="D18" s="48"/>
     </row>
     <row r="19" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="37"/>
-      <c r="B19" s="49" t="s">
+      <c r="A19" s="54"/>
+      <c r="B19" s="22" t="s">
         <v>37</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="40"/>
+      <c r="D19" s="48"/>
     </row>
     <row r="20" spans="1:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="38"/>
+      <c r="A20" s="55"/>
       <c r="B20" s="8" t="s">
         <v>43</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="41"/>
+      <c r="D20" s="49"/>
     </row>
     <row r="21" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="38" t="s">
         <v>48</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1206,30 +1212,30 @@
       <c r="C21" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="30"/>
+      <c r="D21" s="41"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="28"/>
+      <c r="A22" s="39"/>
       <c r="B22" s="3" t="s">
         <v>50</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="31"/>
+      <c r="D22" s="42"/>
     </row>
     <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="29"/>
-      <c r="B23" s="51" t="s">
+      <c r="A23" s="40"/>
+      <c r="B23" s="24" t="s">
         <v>51</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D23" s="32"/>
+      <c r="D23" s="43"/>
     </row>
     <row r="24" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="29" t="s">
         <v>58</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1238,32 +1244,32 @@
       <c r="C24" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="D24" s="32" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="19"/>
+      <c r="A25" s="30"/>
       <c r="B25" s="3" t="s">
         <v>60</v>
       </c>
       <c r="C25" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="22"/>
+      <c r="D25" s="33"/>
     </row>
     <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="20"/>
-      <c r="B26" s="51" t="s">
+      <c r="A26" s="31"/>
+      <c r="B26" s="24" t="s">
         <v>61</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D26" s="23"/>
+      <c r="D26" s="34"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="29" t="s">
         <v>65</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -1272,97 +1278,97 @@
       <c r="C27" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D27" s="39" t="s">
+      <c r="D27" s="47" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="19"/>
+      <c r="A28" s="30"/>
       <c r="B28" s="3" t="s">
         <v>67</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D28" s="40"/>
+      <c r="D28" s="48"/>
     </row>
     <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="20"/>
-      <c r="B29" s="51" t="s">
+      <c r="A29" s="31"/>
+      <c r="B29" s="24" t="s">
         <v>68</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D29" s="41"/>
+      <c r="D29" s="49"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="18" t="s">
+      <c r="A30" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="52" t="s">
+      <c r="B30" s="25" t="s">
         <v>74</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D30" s="42" t="s">
+      <c r="D30" s="50" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="19"/>
-      <c r="B31" s="53" t="s">
+      <c r="A31" s="30"/>
+      <c r="B31" s="26" t="s">
         <v>75</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D31" s="43"/>
+      <c r="D31" s="51"/>
     </row>
     <row r="32" spans="1:4" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="20"/>
-      <c r="B32" s="54" t="s">
+      <c r="A32" s="31"/>
+      <c r="B32" s="27" t="s">
         <v>76</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D32" s="44"/>
+      <c r="D32" s="52"/>
     </row>
     <row r="33" spans="1:4" ht="72.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A33" s="27" t="s">
+      <c r="A33" s="38" t="s">
         <v>82</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C33" s="45" t="s">
+      <c r="C33" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="D33" s="21" t="s">
+      <c r="D33" s="32" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="72.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A34" s="28"/>
+      <c r="A34" s="39"/>
       <c r="B34" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C34" s="47" t="s">
+      <c r="C34" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="D34" s="22"/>
+      <c r="D34" s="33"/>
     </row>
     <row r="35" spans="1:4" ht="52.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="29"/>
-      <c r="B35" s="46" t="s">
+      <c r="A35" s="40"/>
+      <c r="B35" s="19" t="s">
         <v>87</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D35" s="23"/>
+      <c r="D35" s="34"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D38" s="17"/>

</xml_diff>